<commit_message>
ADDED the norm outside temperature to region input
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Region.xlsx
+++ b/data/input_operation/OperationScenario_Component_Region.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B0C5749-51E7-420F-B67C-0D30E13D1152}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392D344A-A97A-4475-8F60-1084D0BB6967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Reg" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID_Region</t>
   </si>
@@ -33,11 +33,14 @@
   <si>
     <t>DE</t>
   </si>
+  <si>
+    <t>norm_outside_temperature</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,14 +874,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -888,8 +893,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -899,6 +907,9 @@
       <c r="C2">
         <v>2019</v>
       </c>
+      <c r="D2">
+        <v>-12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed project name and paths for output and figures
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Region.xlsx
+++ b/data/input_operation/OperationScenario_Component_Region.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3FC732-3A4B-4D94-9D69-400F3C3BB566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67805CD9-DDF5-4E43-AE06-6C6587AE2B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,7 +878,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D2">
         <v>-12</v>

</xml_diff>

<commit_message>
outside temperature set to -17.5 so heating element will not be used
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Region.xlsx
+++ b/data/input_operation/OperationScenario_Component_Region.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67805CD9-DDF5-4E43-AE06-6C6587AE2B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91714FE1-B0C6-465A-B764-2EE7EBE78561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,7 +878,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +908,7 @@
         <v>2018</v>
       </c>
       <c r="D2">
-        <v>-12</v>
+        <v>-17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>